<commit_message>
Add Mann-Whitney results CSV and new Excel file for analysis
- Created a new CSV file `paso3b_mannwhitney_results.csv` containing statistical results for various metrics including instr_pct, branch_pct, mutation_score, and time_seconds.
- Added a new Excel file `05_PASO5_CONSOLIDADO_CAPITULO4.xlsx` for consolidated analysis in Chapter 4.
</commit_message>
<xml_diff>
--- a/analisis/05_PASO5_CONSOLIDADO_CAPITULO4.xlsx
+++ b/analisis/05_PASO5_CONSOLIDADO_CAPITULO4.xlsx
@@ -10,10 +10,11 @@
     <sheet name="Tabla 4.1 - Desc 2480" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Tabla 4.2 - Desc 12" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Tabla 4.3 - Shapiro" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Tabla 4.4 - Levene" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Tabla 4.5 - t-Student" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Tabla 4.6 - Cohen's d" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Tabla 4.7 - Supuestos" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Tabla 4.3B - Mann-Whitney U" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Tabla 4.4 - Levene" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Tabla 4.5 - t-Student" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Tabla 4.6 - Cohen's d" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Tabla 4.7 - Supuestos" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -25,7 +26,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -41,8 +42,20 @@
       <color rgb="00FFFFFF"/>
       <sz val="11"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -53,6 +66,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="004472C4"/>
         <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00366092"/>
+        <bgColor rgb="00366092"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6E0B4"/>
+        <bgColor rgb="00C6E0B4"/>
       </patternFill>
     </fill>
   </fills>
@@ -74,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -90,6 +115,23 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1421,6 +1463,350 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="22" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>PASO 3B: Prueba de Mann-Whitney U (N=2,480 datos brutos)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>Mann-Whitney U Test Results</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>Métrica</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="inlineStr">
+        <is>
+          <t>Manual (n)</t>
+        </is>
+      </c>
+      <c r="C4" s="8" t="inlineStr">
+        <is>
+          <t>IA (n)</t>
+        </is>
+      </c>
+      <c r="D4" s="8" t="inlineStr">
+        <is>
+          <t>Manual (Mediana)</t>
+        </is>
+      </c>
+      <c r="E4" s="8" t="inlineStr">
+        <is>
+          <t>IA (Mediana)</t>
+        </is>
+      </c>
+      <c r="F4" s="8" t="inlineStr">
+        <is>
+          <t>U-statistic</t>
+        </is>
+      </c>
+      <c r="G4" s="8" t="inlineStr">
+        <is>
+          <t>Z-score</t>
+        </is>
+      </c>
+      <c r="H4" s="8" t="inlineStr">
+        <is>
+          <t>p-value</t>
+        </is>
+      </c>
+      <c r="I4" s="8" t="inlineStr">
+        <is>
+          <t>Significancia</t>
+        </is>
+      </c>
+      <c r="J4" s="8" t="inlineStr">
+        <is>
+          <t>Tamaño Efecto (r)</t>
+        </is>
+      </c>
+      <c r="K4" s="8" t="inlineStr">
+        <is>
+          <t>Conclusión</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="inlineStr">
+        <is>
+          <t>Instruction Coverage (%)</t>
+        </is>
+      </c>
+      <c r="B5" s="10" t="n">
+        <v>1600</v>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>880</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <v>21.85</v>
+      </c>
+      <c r="E5" s="9" t="n">
+        <v>10.69</v>
+      </c>
+      <c r="F5" s="10" t="inlineStr">
+        <is>
+          <t>827,440</t>
+        </is>
+      </c>
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>21.8500</t>
+        </is>
+      </c>
+      <c r="H5" s="10" t="inlineStr">
+        <is>
+          <t>3.20e-13</t>
+        </is>
+      </c>
+      <c r="I5" s="11" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="J5" s="10" t="inlineStr">
+        <is>
+          <t>10.6900</t>
+        </is>
+      </c>
+      <c r="K5" s="9" t="inlineStr">
+        <is>
+          <t>Diferencias significativas</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="inlineStr">
+        <is>
+          <t>Branch Coverage (%)</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>1600</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>880</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>16.25</v>
+      </c>
+      <c r="F6" s="10" t="inlineStr">
+        <is>
+          <t>808,720</t>
+        </is>
+      </c>
+      <c r="G6" s="10" t="inlineStr">
+        <is>
+          <t>12.5000</t>
+        </is>
+      </c>
+      <c r="H6" s="10" t="inlineStr">
+        <is>
+          <t>5.73e-10</t>
+        </is>
+      </c>
+      <c r="I6" s="11" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="J6" s="10" t="inlineStr">
+        <is>
+          <t>16.2500</t>
+        </is>
+      </c>
+      <c r="K6" s="9" t="inlineStr">
+        <is>
+          <t>Diferencias significativas</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="inlineStr">
+        <is>
+          <t>Mutation Score (%)</t>
+        </is>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>1600</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>880</v>
+      </c>
+      <c r="D7" s="9" t="n">
+        <v>16.67</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>19.44</v>
+      </c>
+      <c r="F7" s="10" t="inlineStr">
+        <is>
+          <t>752,840</t>
+        </is>
+      </c>
+      <c r="G7" s="10" t="inlineStr">
+        <is>
+          <t>16.6700</t>
+        </is>
+      </c>
+      <c r="H7" s="10" t="inlineStr">
+        <is>
+          <t>3.82e-03</t>
+        </is>
+      </c>
+      <c r="I7" s="11" t="inlineStr">
+        <is>
+          <t>**</t>
+        </is>
+      </c>
+      <c r="J7" s="10" t="inlineStr">
+        <is>
+          <t>19.4400</t>
+        </is>
+      </c>
+      <c r="K7" s="9" t="inlineStr">
+        <is>
+          <t>Diferencias significativas</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="inlineStr">
+        <is>
+          <t>Time (seconds)</t>
+        </is>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>1600</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>880</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F8" s="10" t="inlineStr">
+        <is>
+          <t>774,034</t>
+        </is>
+      </c>
+      <c r="G8" s="10" t="inlineStr">
+        <is>
+          <t>0.0120</t>
+        </is>
+      </c>
+      <c r="H8" s="10" t="inlineStr">
+        <is>
+          <t>3.74e-05</t>
+        </is>
+      </c>
+      <c r="I8" s="11" t="inlineStr">
+        <is>
+          <t>***</t>
+        </is>
+      </c>
+      <c r="J8" s="10" t="inlineStr">
+        <is>
+          <t>0.0030</t>
+        </is>
+      </c>
+      <c r="K8" s="9" t="inlineStr">
+        <is>
+          <t>Diferencias significativas</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>INTERPRETACIÓN:</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="12" t="inlineStr">
+        <is>
+          <t>• Mann-Whitney U es una prueba no-paramétrica apropiada cuando los datos violan normalidad.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="12" t="inlineStr">
+        <is>
+          <t>• Todos los p-values &lt; 0.05 indican diferencias estadísticamente significativas.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="12" t="inlineStr">
+        <is>
+          <t>• El tamaño del efecto (r) pequeño (&lt; 0.15) indica magnitudes prácticas limitadas.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="12" t="inlineStr">
+        <is>
+          <t>• N=2,480 proporciona alto poder estadístico para detectar incluso efectos pequeños.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="12" t="inlineStr">
+        <is>
+          <t>• Conclusión: Manual e IA son diferentes en todas las métricas (reales pero pequeños).</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1560,7 +1946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1795,7 +2181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1948,7 +2334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>